<commit_message>
Updated, now extent reports working fine
</commit_message>
<xml_diff>
--- a/data/getData.xlsx
+++ b/data/getData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SYED SAMEER\eclipse-workspace\SalesAndInventoryTestNg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C6688F-AF27-4B11-8D99-929E5630A246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C907A73-F2E3-4837-8289-0C3B02CA18AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" xr2:uid="{547EC5BD-7D56-48A0-B1AD-536AF6A6E1F2}"/>
   </bookViews>
@@ -52,15 +52,6 @@
     <t>productQuantity</t>
   </si>
   <si>
-    <t>Lalit</t>
-  </si>
-  <si>
-    <t>Pungi</t>
-  </si>
-  <si>
-    <t>Newmen E120</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -73,53 +64,62 @@
     <t>categoryName</t>
   </si>
   <si>
+    <t>supplierName</t>
+  </si>
+  <si>
+    <t>Zepto199</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>5051993</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>productCode</t>
+  </si>
+  <si>
+    <t>onHand</t>
+  </si>
+  <si>
+    <t>029</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>934122</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>life</t>
+  </si>
+  <si>
     <t>Monitor</t>
   </si>
   <si>
-    <t>supplierName</t>
-  </si>
-  <si>
-    <t>Zepto199</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>5051993</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>226628</t>
-  </si>
-  <si>
-    <t>productCode</t>
-  </si>
-  <si>
-    <t>onHand</t>
-  </si>
-  <si>
-    <t>029</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>145</t>
+    <t>Newmen E120360</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +145,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF36B9CC"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -166,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -181,6 +187,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +505,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,15 +535,15 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -544,71 +551,71 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>